<commit_message>
Change DRV8824 interface mode from 2-Pin to 4-Pin
* MOD: Drop ENC_2A, B (use only left motor encoder)
</commit_message>
<xml_diff>
--- a/JLCSMT_BOM.xlsx
+++ b/JLCSMT_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Jeonghyun\graduate-project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Jeonghyun\gradproj\RBFPID-Balbot-circuit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE30A764-9875-427B-975F-FA31FAA17731}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CDECE1A-4B33-462B-A717-40D6F8A812DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8415" yWindow="6075" windowWidth="12150" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>Comment</t>
   </si>
@@ -162,12 +162,24 @@
     <t>C98220</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
+  <si>
+    <t>0.1uF</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>C2</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>C1591</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -210,6 +222,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -219,7 +238,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -242,13 +261,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -275,6 +305,15 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -621,8 +660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -731,6 +770,20 @@
         <v>15</v>
       </c>
     </row>
+    <row r="8" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A8" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
     <row r="9" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A9"/>
     </row>

</xml_diff>